<commit_message>
revise missing fields for CPR report
</commit_message>
<xml_diff>
--- a/CPR_Missing_Fields.xlsx
+++ b/CPR_Missing_Fields.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Mising field</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Claims_Officer_Name</t>
-  </si>
-  <si>
     <t>EMPL_SIZE</t>
   </si>
   <si>
@@ -86,28 +80,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CLAIMS_OFFICERS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / First_Name &amp; Last_Name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>POLICY_TERM_DETAIL</t>
     </r>
     <r>
@@ -240,37 +212,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">CLAIMS_OFFICERS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Grp</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">CLAIM_DETAIL </t>
     </r>
     <r>
@@ -437,9 +378,6 @@
       </rPr>
       <t xml:space="preserve"> / Deemed_HoursPerWeek</t>
     </r>
-  </si>
-  <si>
-    <t>Entitlement_Weeks</t>
   </si>
   <si>
     <t>Missing fields of CPR Summary Report</t>
@@ -491,16 +429,13 @@
     <t>Need 2 columns from 2 different tables:
 - Column DESCRIPTION from ANZSIC 
 - And column Tariff from ACTIVITY_DETAIL_AUDIT</t>
-  </si>
-  <si>
-    <t>Calculate the entitlement weeks value for each claim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,12 +454,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -563,11 +492,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,11 +799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,21 +814,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,14 +844,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -931,18 +863,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,7 +895,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -974,7 +903,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -982,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,7 +919,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +927,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,47 +935,23 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>